<commit_message>
Server-Schnittstelle um Server-Check erweitert.
Aufruf über context root.
</commit_message>
<xml_diff>
--- a/Documents/Concept/Schnittstelle_Server.xlsx
+++ b/Documents/Concept/Schnittstelle_Server.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="77">
   <si>
     <t>Context Root:</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>wi_quiz/</t>
   </si>
   <si>
     <t>logout</t>
@@ -276,6 +273,21 @@
   </si>
   <si>
     <t>user/statistics</t>
+  </si>
+  <si>
+    <t>Studiduell/</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>text/html</t>
+  </si>
+  <si>
+    <t>Erfolgsmeldung, wenn ReST-Webservice verfügbar ist.</t>
+  </si>
+  <si>
+    <t>Prüfung, ob ReST-Webservice erreichbar ist.</t>
   </si>
 </sst>
 </file>
@@ -350,7 +362,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
     <dxf>
@@ -412,7 +424,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="A4:M19" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="A4:M20" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <tableColumns count="13">
     <tableColumn id="1" name="Resource" dataDxfId="12"/>
     <tableColumn id="2" name="Param1" dataDxfId="11"/>
@@ -433,9 +445,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -473,7 +485,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -545,7 +557,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -719,14 +731,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
@@ -742,7 +755,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -774,482 +787,505 @@
         <v>9</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="J5" s="1"/>
       <c r="K5" s="1" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="I6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J6" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="K6" s="1" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="L8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="I9" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="I11" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L11" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="L12" s="1"/>
-      <c r="M12" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="I13" s="1" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="M13" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="D14" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="I14" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J14" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="K14" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="D15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>52</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="J15" s="1"/>
       <c r="K15" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="I16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J16" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="K16" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="J17" s="1"/>
       <c r="K17" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="I18" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J18" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="K18" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" ht="195" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
+      <c r="K19" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" ht="195" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1266,7 +1302,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1278,7 +1314,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fortschritt in der Schnittstbeschr. aktualisiert.
</commit_message>
<xml_diff>
--- a/Documents/Concept/Schnittstelle_Server.xlsx
+++ b/Documents/Concept/Schnittstelle_Server.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="84">
   <si>
     <t>Context Root:</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Freundesliste</t>
   </si>
   <si>
-    <t>[freund_name]</t>
-  </si>
-  <si>
     <t>Übertragt die Freundesliste</t>
   </si>
   <si>
@@ -123,25 +120,13 @@
     <t>Freund entfernen</t>
   </si>
   <si>
-    <t>searched_nick</t>
-  </si>
-  <si>
     <t>Ergebnisliste</t>
   </si>
   <si>
-    <t>[spieler_name]</t>
-  </si>
-  <si>
     <t>Liste gefundener Mitspieler, deren Name die gesuchte Phrase enthält (like '%abc%')</t>
   </si>
   <si>
-    <t>Name des Gegners</t>
-  </si>
-  <si>
     <t>Um Popup 'Du spielst mit …' anzuzeigen</t>
-  </si>
-  <si>
-    <t>"Hans123"</t>
   </si>
   <si>
     <t>Synchronisieren der Daten des Hauptmenüs (Aktive Spiele und Pending Spiele)
@@ -185,15 +170,6 @@
 UND
 Accept: Spielstatus ACTIVE
 Decline: Spielstatus DECLINED</t>
-  </si>
-  <si>
-    <t>[ {
- categorie_name : {
-  [frage : {
-   // Fragenattribute
-  } ]
- }
-} ]</t>
   </si>
   <si>
     <t>Liefert aus der Schnittmenge 3 zufällige Kategorien inkl. je 3 Fragen</t>
@@ -209,97 +185,135 @@
 er sendet an Gegenspieler Push-Benachrichtigung.</t>
   </si>
   <si>
+    <t>Der Spieler erhält die letzten Fragen des Gegners plus dessen Antworten.</t>
+  </si>
+  <si>
+    <t>settings/set_categories</t>
+  </si>
+  <si>
+    <t>settings/unfriend</t>
+  </si>
+  <si>
+    <t>user/search</t>
+  </si>
+  <si>
+    <t>game/create_game_random_opponent</t>
+  </si>
+  <si>
+    <t>game/create_game</t>
+  </si>
+  <si>
+    <t>game/get_game_overview</t>
+  </si>
+  <si>
+    <t>game/answer_duell_request</t>
+  </si>
+  <si>
+    <t>game/get_random_categories</t>
+  </si>
+  <si>
+    <t>game/send_round_result</t>
+  </si>
+  <si>
+    <t>game/continue_round</t>
+  </si>
+  <si>
+    <t>user/statistics</t>
+  </si>
+  <si>
+    <t>Studiduell/</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>text/html</t>
+  </si>
+  <si>
+    <t>Prüfung, ob ReST-Webservice erreichbar ist.</t>
+  </si>
+  <si>
+    <t>Kommentar</t>
+  </si>
+  <si>
+    <t>Umgesetzt</t>
+  </si>
+  <si>
+    <t>nein</t>
+  </si>
+  <si>
+    <t>ja</t>
+  </si>
+  <si>
+    <t>Mock</t>
+  </si>
+  <si>
+    <t>settings/friend</t>
+  </si>
+  <si>
+    <t>Freund hinzufügen</t>
+  </si>
+  <si>
+    <t>settings/list_friends</t>
+  </si>
+  <si>
+    <t>{games:[Spiel_DS]}</t>
+  </si>
+  <si>
+    <t>Statusmeldung, ob Server-Konfiguration korrekt (ReST-WS + DB verfügbar)
+Gibt eine HTML-Seite zurück</t>
+  </si>
+  <si>
+    <t>{users:[user_name]}</t>
+  </si>
+  <si>
+    <t>searched_nick_part</t>
+  </si>
+  <si>
+    <t>Name des Gegners oder null</t>
+  </si>
+  <si>
+    <t>{user:Hans_Wurst}
+ALTERNATIV:
+{user:null} (null nicht in Hochkommata)</t>
+  </si>
+  <si>
     <t>{
- [frage : {
+ [question : {
   // Fragenattribute
  }],
- [antwort : {
+ [answer : {
   // Antworten des Gegners
  }],
 }</t>
   </si>
   <si>
-    <t>Der Spieler erhält die letzten Fragen des Gegners plus dessen Antworten.</t>
-  </si>
-  <si>
     <t>{
- spiel : {
-  verloren : x,
-  gewonnen : x,
-  unentschieden : x,
+ game : {
+  lost : x,
+  won : x,
+  draw : x,
   total : x
  },
- fragen : {
-  proz_richtig : x,
+ questions : {
+  perc_right : x,
   total : x
  }
 }</t>
   </si>
   <si>
-    <t>settings/set_categories</t>
-  </si>
-  <si>
-    <t>settings/get_friends_list</t>
-  </si>
-  <si>
-    <t>settings/unfriend</t>
-  </si>
-  <si>
-    <t>user/search</t>
-  </si>
-  <si>
-    <t>game/create_game_random_opponent</t>
-  </si>
-  <si>
-    <t>game/create_game</t>
-  </si>
-  <si>
-    <t>game/get_game_overview</t>
-  </si>
-  <si>
-    <t>game/answer_duell_request</t>
-  </si>
-  <si>
-    <t>game/get_random_categories</t>
-  </si>
-  <si>
-    <t>game/send_round_result</t>
-  </si>
-  <si>
-    <t>game/continue_round</t>
-  </si>
-  <si>
-    <t>user/statistics</t>
-  </si>
-  <si>
-    <t>Studiduell/</t>
-  </si>
-  <si>
-    <t>GET</t>
-  </si>
-  <si>
-    <t>text/html</t>
-  </si>
-  <si>
-    <t>Prüfung, ob ReST-Webservice erreichbar ist.</t>
-  </si>
-  <si>
-    <t>Statusmeldung, ob Server-Konfiguration korrekt (ReST-WS + DB verfügbar)</t>
-  </si>
-  <si>
-    <t>Kommentar</t>
-  </si>
-  <si>
-    <t>Umgesetzt</t>
-  </si>
-  <si>
-    <t>nein</t>
-  </si>
-  <si>
-    <t>ja</t>
-  </si>
-  <si>
-    <t>Mock</t>
+    <t>[ {
+ categorie_name : {
+  [question : {
+   // Fragenattribute
+  } ]
+ }
+} ]</t>
+  </si>
+  <si>
+    <t>{friends:[friend_name]}
+ALTERNATIV:
+{friends:null}</t>
   </si>
 </sst>
 </file>
@@ -439,7 +453,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="A4:N20" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="A4:N21" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <tableColumns count="14">
     <tableColumn id="1" name="Resource" dataDxfId="13"/>
     <tableColumn id="2" name="Param1" dataDxfId="12"/>
@@ -747,22 +761,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="35.28515625" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" customWidth="1"/>
     <col min="11" max="11" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -771,7 +785,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -812,13 +826,13 @@
         <v>24</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -826,22 +840,22 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>75</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -875,7 +889,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="90" x14ac:dyDescent="0.25">
@@ -900,16 +914,18 @@
         <v>17</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="K7" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -945,12 +961,12 @@
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>12</v>
@@ -981,12 +997,12 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>12</v>
@@ -1007,20 +1023,20 @@
         <v>30</v>
       </c>
       <c r="J10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>12</v>
@@ -1029,7 +1045,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1037,7 +1053,7 @@
         <v>14</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>20</v>
@@ -1046,58 +1062,60 @@
         <v>19</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L12" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1105,28 +1123,26 @@
         <v>14</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="L13" s="1"/>
-      <c r="M13" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="M13" s="1"/>
       <c r="N13" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="135" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>12</v>
@@ -1134,35 +1150,35 @@
       <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
+      <c r="M14" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="N14" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>12</v>
@@ -1171,7 +1187,7 @@
         <v>13</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1179,24 +1195,26 @@
         <v>14</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J15" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="K15" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>12</v>
@@ -1205,135 +1223,137 @@
         <v>13</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>50</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="J16" s="1"/>
       <c r="K16" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J17" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="K17" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="J18" s="1"/>
       <c r="K18" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J19" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="K19" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="195" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1344,19 +1364,51 @@
         <v>17</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
+      <c r="K20" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1" t="s">
-        <v>78</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="195" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N5:N20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N5:N21">
       <formula1>"nein,ja,Mock"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>